<commit_message>
Removed input borders and added advanced sample form.
</commit_message>
<xml_diff>
--- a/extras/sample-form/Table grid field plug-in advanced sample form.xlsx
+++ b/extras/sample-form/Table grid field plug-in advanced sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitoworks/Downloads/GitHub/table-grid/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E52A38-09B2-9048-9004-E09AC2DE9B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB50EF6C-1B9E-FA4B-9BF0-1C76A4A5D1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="1480" windowWidth="23240" windowHeight="12440" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="420">
   <si>
     <t>type</t>
   </si>
@@ -2630,16 +2630,125 @@
     <t>The answer is: ${crops}</t>
   </si>
   <si>
-    <t>custom-table-grid(data_type="number", columns=4, rows=4, column_headers="Maize|Sorghum|Millet|Rice", row_headers="Area Planted|Produced|Quantity sold|Quantity given away")</t>
-  </si>
-  <si>
     <t>Advanced sample form - table grid</t>
   </si>
   <si>
     <t>advanced_table_grid</t>
   </si>
   <si>
-    <t>select_multple crops</t>
+    <t>select_multiple crops</t>
+  </si>
+  <si>
+    <t>crops_grown</t>
+  </si>
+  <si>
+    <t>Which of these crops do you grow?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>num_crops_selected</t>
+  </si>
+  <si>
+    <t>if(selected(${crops_grown}, '-1'),
+count-selected(${crops_grown}) - 1,
+count-selected(${crops_grown}))</t>
+  </si>
+  <si>
+    <t>other_crops_gr</t>
+  </si>
+  <si>
+    <t>Other crops grown</t>
+  </si>
+  <si>
+    <t>selected(${crops_grown}, '-1')</t>
+  </si>
+  <si>
+    <t>num_other</t>
+  </si>
+  <si>
+    <t>How many other crops do you grow?</t>
+  </si>
+  <si>
+    <t>. &gt; 0</t>
+  </si>
+  <si>
+    <t>Make sure you enter a number greater than 0, or go back an un-select "Other".</t>
+  </si>
+  <si>
+    <t>other_crops_rep</t>
+  </si>
+  <si>
+    <t>Enter other crops</t>
+  </si>
+  <si>
+    <t>index() &lt;= ${num_other}</t>
+  </si>
+  <si>
+    <t>${num_other}</t>
+  </si>
+  <si>
+    <t>other_crop_index</t>
+  </si>
+  <si>
+    <t>other_crop_name</t>
+  </si>
+  <si>
+    <t>What is the name of crop ${other_crop_index}?</t>
+  </si>
+  <si>
+    <t>num_crops</t>
+  </si>
+  <si>
+    <t>${num_crops_selected} + coalesce(${num_other}, 0)</t>
+  </si>
+  <si>
+    <t>crop_list</t>
+  </si>
+  <si>
+    <t>Crop list</t>
+  </si>
+  <si>
+    <t>index() &lt;= ${num_crops}</t>
+  </si>
+  <si>
+    <t>${num_crops}</t>
+  </si>
+  <si>
+    <t>crop_index</t>
+  </si>
+  <si>
+    <t>crop_name</t>
+  </si>
+  <si>
+    <t>if(${crop_index} &lt;= ${num_crops_selected},
+choice-label(${crops_grown}, selected-at(${crops_grown}, ${crop_index} - 1)),
+indexed-repeat(${other_crop_name}, ${other_crops_rep}, ${crop_index} - ${num_crops_selected}))</t>
+  </si>
+  <si>
+    <t>crop_names</t>
+  </si>
+  <si>
+    <t>Apples</t>
+  </si>
+  <si>
+    <t>Bananas</t>
+  </si>
+  <si>
+    <t>Carrots</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>join('|', ${crop_name})</t>
+  </si>
+  <si>
+    <t>custom-table-grid(columns=${num_crops}, rows=4, column_headers=${crop_names}, row_headers="Area Planted|Produced|Quantity sold|Quantity given away")</t>
   </si>
 </sst>
 </file>
@@ -5464,11 +5573,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF16"/>
+  <dimension ref="A1:AF29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5486,7 +5595,7 @@
     <col min="11" max="11" width="8.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="18" style="9" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="9.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.5" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.33203125" style="9" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="15" style="9" customWidth="1" collapsed="1"/>
     <col min="16" max="17" width="48" style="9" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="10.83203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5701,86 +5810,301 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>384</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>385</v>
       </c>
       <c r="D13" s="53"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K13" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>387</v>
+      </c>
       <c r="D14" s="53"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
+      <c r="N14" s="11" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="D15" s="53"/>
+      <c r="I15" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="D16" s="53"/>
+      <c r="G16" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="D17" s="53"/>
+      <c r="I17" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="O17" s="9" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="D18" s="53"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="N18" s="9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B19" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="D20" s="53"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="D21" s="53"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="D22" s="53"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="N22" s="9" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="D23" s="53"/>
+      <c r="I23" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="O23" s="9" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="N24" s="9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="170" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="D25" s="53"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="N25" s="11" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="D26" s="53"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="D27" s="53"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="N27" s="9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C28" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D28" t="s">
         <v>374</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="F28" s="9" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>380</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B1:C14 F1:F14 I1:I14 B17:C1048576 I17:I1048576 F17:F1048576">
+  <conditionalFormatting sqref="B1:C27 F1:F27 I1:I27 B30:C1048576 I30:I1048576 F30:F1048576">
     <cfRule type="expression" dxfId="221" priority="2317" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C14 I1:I14 B17:C1048576 I17:I1048576">
+  <conditionalFormatting sqref="B1:C27 I1:I27 B30:C1048576 I30:I1048576">
     <cfRule type="expression" dxfId="220" priority="2314" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D14 F1:F14 B17:D1048576 F17:F1048576">
+  <conditionalFormatting sqref="B1:D27 F1:F27 B30:D1048576 F30:F1048576">
     <cfRule type="expression" dxfId="219" priority="2311" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D14 G1:H14 B17:D1048576 G17:H1048576">
+  <conditionalFormatting sqref="B1:D27 G1:H27 B30:D1048576 G30:H1048576">
     <cfRule type="expression" dxfId="218" priority="2309" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D14 G1:H14 B17:D1048576 G17:H1048576">
+  <conditionalFormatting sqref="B1:D27 G1:H27 B30:D1048576 G30:H1048576">
     <cfRule type="expression" dxfId="217" priority="2307" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C14 F1:F14 B17:C1048576 F17:F1048576">
+  <conditionalFormatting sqref="B1:C27 F1:F27 B30:C1048576 F30:F1048576">
     <cfRule type="expression" dxfId="216" priority="2302" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B14 F1:F14 F17:F1048576 B17:B1048576">
+  <conditionalFormatting sqref="B1:B27 F1:F27 F30:F1048576 B30:B1048576">
     <cfRule type="expression" dxfId="215" priority="2292" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C14 B17:C1048576">
+  <conditionalFormatting sqref="B1:C27 B30:C1048576">
     <cfRule type="expression" dxfId="214" priority="2286" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
@@ -5791,27 +6115,27 @@
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B14 B17:B1048576">
+  <conditionalFormatting sqref="B1:B27 B30:B1048576">
     <cfRule type="expression" dxfId="211" priority="2284" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C14 F1:F14 B17:C1048576 F17:F1048576">
+  <conditionalFormatting sqref="B1:C27 F1:F27 B30:C1048576 F30:F1048576">
     <cfRule type="expression" dxfId="210" priority="2282" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C14 F1:F14 B17:C1048576 F17:F1048576">
+  <conditionalFormatting sqref="B1:C27 F1:F27 B30:C1048576 F30:F1048576">
     <cfRule type="expression" dxfId="209" priority="2278" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C14 B17:C1048576">
+  <conditionalFormatting sqref="B1:C27 B30:C1048576">
     <cfRule type="expression" dxfId="208" priority="2276" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:S14 A17:S1048576">
+  <conditionalFormatting sqref="A1:S27 A30:S1048576">
     <cfRule type="expression" dxfId="207" priority="2270" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
@@ -5870,338 +6194,338 @@
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B14 B17:B1048576">
+  <conditionalFormatting sqref="B1:B27 B30:B1048576">
     <cfRule type="expression" dxfId="188" priority="2271" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F14 B1:B14 B17:B1048576 F17:F1048576">
+  <conditionalFormatting sqref="F1:F27 B1:B27 B30:B1048576 F30:F1048576">
     <cfRule type="expression" dxfId="187" priority="2269" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 F15:F16 I15:I16 B16:C16">
+  <conditionalFormatting sqref="B28 F28:F29 I28:I29 B29:C29">
     <cfRule type="expression" dxfId="186" priority="175" stopIfTrue="1">
-      <formula>$A15="begin group"</formula>
+      <formula>$A28="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 I15:I16 B16:C16">
+  <conditionalFormatting sqref="B28 I28:I29 B29:C29">
     <cfRule type="expression" dxfId="185" priority="172" stopIfTrue="1">
-      <formula>$A15="begin repeat"</formula>
+      <formula>$A28="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 F15:F16 B16:D16">
+  <conditionalFormatting sqref="B28 F28:F29 B29:D29">
     <cfRule type="expression" dxfId="184" priority="169" stopIfTrue="1">
-      <formula>$A15="text"</formula>
+      <formula>$A28="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 G15:H16 B16:D16">
+  <conditionalFormatting sqref="B28 G28:H29 B29:D29">
     <cfRule type="expression" dxfId="183" priority="167" stopIfTrue="1">
-      <formula>$A15="integer"</formula>
+      <formula>$A28="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 G15:H16 B16:D16">
+  <conditionalFormatting sqref="B28 G28:H29 B29:D29">
     <cfRule type="expression" dxfId="182" priority="165" stopIfTrue="1">
-      <formula>$A15="decimal"</formula>
+      <formula>$A28="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 F15:F16 B16:C16">
+  <conditionalFormatting sqref="B28 F28:F29 B29:C29">
     <cfRule type="expression" dxfId="181" priority="163" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A15, 16)="select_multiple ", LEN($A15)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A15, 17)))), AND(LEFT($A15, 11)="select_one ", LEN($A15)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A15, 12)))))</formula>
+      <formula>OR(AND(LEFT($A28, 16)="select_multiple ", LEN($A28)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A28, 17)))), AND(LEFT($A28, 11)="select_one ", LEN($A28)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A28, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B16 F15:F16">
+  <conditionalFormatting sqref="B28:B29 F28:F29">
     <cfRule type="expression" dxfId="180" priority="160" stopIfTrue="1">
-      <formula>OR($A15="audio audit", $A15="text audit", $A15="speed violations count", $A15="speed violations list", $A15="speed violations audit")</formula>
+      <formula>OR($A28="audio audit", $A28="text audit", $A28="speed violations count", $A28="speed violations list", $A28="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 B16:C16">
+  <conditionalFormatting sqref="B28 B29:C29">
     <cfRule type="expression" dxfId="179" priority="154" stopIfTrue="1">
-      <formula>$A15="note"</formula>
+      <formula>$A28="note"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="178" priority="156" stopIfTrue="1">
-      <formula>$A15="barcode"</formula>
+      <formula>$A28="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="177" priority="158" stopIfTrue="1">
-      <formula>OR($A15="geopoint", $A15="geoshape", $A15="geotrace")</formula>
+      <formula>OR($A28="geopoint", $A28="geoshape", $A28="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B16">
+  <conditionalFormatting sqref="B28:B29">
     <cfRule type="expression" dxfId="176" priority="152" stopIfTrue="1">
-      <formula>OR($A15="calculate", $A15="calculate_here")</formula>
+      <formula>OR($A28="calculate", $A28="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 F15:F16 B16:C16">
+  <conditionalFormatting sqref="B28 F28:F29 B29:C29">
     <cfRule type="expression" dxfId="175" priority="150" stopIfTrue="1">
-      <formula>OR($A15="date", $A15="datetime")</formula>
+      <formula>OR($A28="date", $A28="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 F15:F16 B16:C16">
+  <conditionalFormatting sqref="B28 F28:F29 B29:C29">
     <cfRule type="expression" dxfId="174" priority="148" stopIfTrue="1">
-      <formula>$A15="image"</formula>
+      <formula>$A28="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 B16:C16">
+  <conditionalFormatting sqref="B28 B29:C29">
     <cfRule type="expression" dxfId="173" priority="146" stopIfTrue="1">
-      <formula>OR($A15="audio", $A15="video")</formula>
+      <formula>OR($A28="audio", $A28="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:B15 N15:S16 E15:M15 A16:M16">
+  <conditionalFormatting sqref="A28:B28 N28:S29 E28:M28 A29:M29">
     <cfRule type="expression" dxfId="172" priority="143" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A15, 14)="sensor_stream ", LEN($A15)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A15, 15)))), AND(LEFT($A15, 17)="sensor_statistic ", LEN($A15)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A15, 18)))))</formula>
+      <formula>OR(AND(LEFT($A28, 14)="sensor_stream ", LEN($A28)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A28, 15)))), AND(LEFT($A28, 17)="sensor_statistic ", LEN($A28)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A28, 18)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="171" priority="145" stopIfTrue="1">
-      <formula>$A15="comments"</formula>
+      <formula>$A28="comments"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="170" priority="147" stopIfTrue="1">
-      <formula>OR($A15="audio", $A15="video")</formula>
+      <formula>OR($A28="audio", $A28="video")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="169" priority="149" stopIfTrue="1">
-      <formula>$A15="image"</formula>
+      <formula>$A28="image"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="168" priority="151" stopIfTrue="1">
-      <formula>OR($A15="date", $A15="datetime")</formula>
+      <formula>OR($A28="date", $A28="datetime")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="167" priority="153" stopIfTrue="1">
-      <formula>OR($A15="calculate", $A15="calculate_here")</formula>
+      <formula>OR($A28="calculate", $A28="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="166" priority="155" stopIfTrue="1">
-      <formula>$A15="note"</formula>
+      <formula>$A28="note"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="165" priority="157" stopIfTrue="1">
-      <formula>$A15="barcode"</formula>
+      <formula>$A28="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="164" priority="159" stopIfTrue="1">
-      <formula>OR($A15="geopoint", $A15="geoshape", $A15="geotrace")</formula>
+      <formula>OR($A28="geopoint", $A28="geoshape", $A28="geotrace")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="163" priority="161" stopIfTrue="1">
-      <formula>OR($A15="audio audit", $A15="text audit", $A15="speed violations count", $A15="speed violations list", $A15="speed violations audit")</formula>
+      <formula>OR($A28="audio audit", $A28="text audit", $A28="speed violations count", $A28="speed violations list", $A28="speed violations audit")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="162" priority="162" stopIfTrue="1">
-      <formula>OR($A15="username", $A15="phonenumber", $A15="start", $A15="end", $A15="deviceid", $A15="subscriberid", $A15="simserial", $A15="caseid")</formula>
+      <formula>OR($A28="username", $A28="phonenumber", $A28="start", $A28="end", $A28="deviceid", $A28="subscriberid", $A28="simserial", $A28="caseid")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="161" priority="164" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A15, 16)="select_multiple ", LEN($A15)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A15, 17)))), AND(LEFT($A15, 11)="select_one ", LEN($A15)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A15, 12)))))</formula>
+      <formula>OR(AND(LEFT($A28, 16)="select_multiple ", LEN($A28)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A28, 17)))), AND(LEFT($A28, 11)="select_one ", LEN($A28)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A28, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="160" priority="166" stopIfTrue="1">
-      <formula>$A15="decimal"</formula>
+      <formula>$A28="decimal"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="159" priority="168" stopIfTrue="1">
-      <formula>$A15="integer"</formula>
+      <formula>$A28="integer"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="158" priority="170" stopIfTrue="1">
-      <formula>$A15="text"</formula>
+      <formula>$A28="text"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="157" priority="171" stopIfTrue="1">
-      <formula>$A15="end repeat"</formula>
+      <formula>$A28="end repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="156" priority="173" stopIfTrue="1">
-      <formula>$A15="begin repeat"</formula>
+      <formula>$A28="begin repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="155" priority="174" stopIfTrue="1">
-      <formula>$A15="end group"</formula>
+      <formula>$A28="end group"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="154" priority="176" stopIfTrue="1">
-      <formula>$A15="begin group"</formula>
+      <formula>$A28="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B16">
+  <conditionalFormatting sqref="B28:B29">
     <cfRule type="expression" dxfId="153" priority="144" stopIfTrue="1">
-      <formula>$A15="comments"</formula>
+      <formula>$A28="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F16 B15:B16">
+  <conditionalFormatting sqref="F28:F29 B28:B29">
     <cfRule type="expression" dxfId="152" priority="142" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A15, 14)="sensor_stream ", LEN($A15)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A15, 15)))), AND(LEFT($A15, 17)="sensor_statistic ", LEN($A15)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A15, 18)))))</formula>
+      <formula>OR(AND(LEFT($A28, 14)="sensor_stream ", LEN($A28)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A28, 15)))), AND(LEFT($A28, 17)="sensor_statistic ", LEN($A28)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A28, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="151" priority="140" stopIfTrue="1">
-      <formula>$A15="begin group"</formula>
+      <formula>$A28="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="150" priority="137" stopIfTrue="1">
-      <formula>$A15="begin repeat"</formula>
+      <formula>$A28="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="149" priority="134" stopIfTrue="1">
-      <formula>$A15="text"</formula>
+      <formula>$A28="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="148" priority="132" stopIfTrue="1">
-      <formula>$A15="integer"</formula>
+      <formula>$A28="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="147" priority="130" stopIfTrue="1">
-      <formula>$A15="decimal"</formula>
+      <formula>$A28="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="146" priority="128" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A15, 16)="select_multiple ", LEN($A15)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A15, 17)))), AND(LEFT($A15, 11)="select_one ", LEN($A15)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A15, 12)))))</formula>
+      <formula>OR(AND(LEFT($A28, 16)="select_multiple ", LEN($A28)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A28, 17)))), AND(LEFT($A28, 11)="select_one ", LEN($A28)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A28, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="145" priority="120" stopIfTrue="1">
-      <formula>$A15="note"</formula>
+      <formula>$A28="note"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="144" priority="122" stopIfTrue="1">
-      <formula>$A15="barcode"</formula>
+      <formula>$A28="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="143" priority="124" stopIfTrue="1">
-      <formula>OR($A15="geopoint", $A15="geoshape", $A15="geotrace")</formula>
+      <formula>OR($A28="geopoint", $A28="geoshape", $A28="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="142" priority="117" stopIfTrue="1">
-      <formula>OR($A15="date", $A15="datetime")</formula>
+      <formula>OR($A28="date", $A28="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="141" priority="115" stopIfTrue="1">
-      <formula>$A15="image"</formula>
+      <formula>$A28="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="140" priority="113" stopIfTrue="1">
-      <formula>OR($A15="audio", $A15="video")</formula>
+      <formula>OR($A28="audio", $A28="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="139" priority="111" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A15, 14)="sensor_stream ", LEN($A15)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A15, 15)))), AND(LEFT($A15, 17)="sensor_statistic ", LEN($A15)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A15, 18)))))</formula>
+      <formula>OR(AND(LEFT($A28, 14)="sensor_stream ", LEN($A28)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A28, 15)))), AND(LEFT($A28, 17)="sensor_statistic ", LEN($A28)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A28, 18)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="138" priority="112" stopIfTrue="1">
-      <formula>$A15="comments"</formula>
+      <formula>$A28="comments"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="137" priority="114" stopIfTrue="1">
-      <formula>OR($A15="audio", $A15="video")</formula>
+      <formula>OR($A28="audio", $A28="video")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="136" priority="116" stopIfTrue="1">
-      <formula>$A15="image"</formula>
+      <formula>$A28="image"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="135" priority="118" stopIfTrue="1">
-      <formula>OR($A15="date", $A15="datetime")</formula>
+      <formula>OR($A28="date", $A28="datetime")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="134" priority="119" stopIfTrue="1">
-      <formula>OR($A15="calculate", $A15="calculate_here")</formula>
+      <formula>OR($A28="calculate", $A28="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="133" priority="121" stopIfTrue="1">
-      <formula>$A15="note"</formula>
+      <formula>$A28="note"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="132" priority="123" stopIfTrue="1">
-      <formula>$A15="barcode"</formula>
+      <formula>$A28="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="131" priority="125" stopIfTrue="1">
-      <formula>OR($A15="geopoint", $A15="geoshape", $A15="geotrace")</formula>
+      <formula>OR($A28="geopoint", $A28="geoshape", $A28="geotrace")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="130" priority="126" stopIfTrue="1">
-      <formula>OR($A15="audio audit", $A15="text audit", $A15="speed violations count", $A15="speed violations list", $A15="speed violations audit")</formula>
+      <formula>OR($A28="audio audit", $A28="text audit", $A28="speed violations count", $A28="speed violations list", $A28="speed violations audit")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="129" priority="127" stopIfTrue="1">
-      <formula>OR($A15="username", $A15="phonenumber", $A15="start", $A15="end", $A15="deviceid", $A15="subscriberid", $A15="simserial", $A15="caseid")</formula>
+      <formula>OR($A28="username", $A28="phonenumber", $A28="start", $A28="end", $A28="deviceid", $A28="subscriberid", $A28="simserial", $A28="caseid")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="128" priority="129" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A15, 16)="select_multiple ", LEN($A15)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A15, 17)))), AND(LEFT($A15, 11)="select_one ", LEN($A15)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A15, 12)))))</formula>
+      <formula>OR(AND(LEFT($A28, 16)="select_multiple ", LEN($A28)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A28, 17)))), AND(LEFT($A28, 11)="select_one ", LEN($A28)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A28, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="127" priority="131" stopIfTrue="1">
-      <formula>$A15="decimal"</formula>
+      <formula>$A28="decimal"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="126" priority="133" stopIfTrue="1">
-      <formula>$A15="integer"</formula>
+      <formula>$A28="integer"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="125" priority="135" stopIfTrue="1">
-      <formula>$A15="text"</formula>
+      <formula>$A28="text"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="124" priority="136" stopIfTrue="1">
-      <formula>$A15="end repeat"</formula>
+      <formula>$A28="end repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="123" priority="138" stopIfTrue="1">
-      <formula>$A15="begin repeat"</formula>
+      <formula>$A28="begin repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="122" priority="139" stopIfTrue="1">
-      <formula>$A15="end group"</formula>
+      <formula>$A28="end group"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="121" priority="141" stopIfTrue="1">
-      <formula>$A15="begin group"</formula>
+      <formula>$A28="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="D28">
     <cfRule type="expression" dxfId="120" priority="105" stopIfTrue="1">
-      <formula>$A15="text"</formula>
+      <formula>$A28="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="D28">
     <cfRule type="expression" dxfId="119" priority="103" stopIfTrue="1">
-      <formula>$A15="integer"</formula>
+      <formula>$A28="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="D28">
     <cfRule type="expression" dxfId="118" priority="101" stopIfTrue="1">
-      <formula>$A15="decimal"</formula>
+      <formula>$A28="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="D28">
     <cfRule type="expression" dxfId="117" priority="89" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A15, 14)="sensor_stream ", LEN($A15)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A15, 15)))), AND(LEFT($A15, 17)="sensor_statistic ", LEN($A15)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A15, 18)))))</formula>
+      <formula>OR(AND(LEFT($A28, 14)="sensor_stream ", LEN($A28)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A28, 15)))), AND(LEFT($A28, 17)="sensor_statistic ", LEN($A28)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A28, 18)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="116" priority="90" stopIfTrue="1">
-      <formula>$A15="comments"</formula>
+      <formula>$A28="comments"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="115" priority="91" stopIfTrue="1">
-      <formula>OR($A15="audio", $A15="video")</formula>
+      <formula>OR($A28="audio", $A28="video")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="114" priority="92" stopIfTrue="1">
-      <formula>$A15="image"</formula>
+      <formula>$A28="image"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="113" priority="93" stopIfTrue="1">
-      <formula>OR($A15="date", $A15="datetime")</formula>
+      <formula>OR($A28="date", $A28="datetime")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="112" priority="94" stopIfTrue="1">
-      <formula>OR($A15="calculate", $A15="calculate_here")</formula>
+      <formula>OR($A28="calculate", $A28="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="111" priority="95" stopIfTrue="1">
-      <formula>$A15="note"</formula>
+      <formula>$A28="note"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="110" priority="96" stopIfTrue="1">
-      <formula>$A15="barcode"</formula>
+      <formula>$A28="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="109" priority="97" stopIfTrue="1">
-      <formula>OR($A15="geopoint", $A15="geoshape", $A15="geotrace")</formula>
+      <formula>OR($A28="geopoint", $A28="geoshape", $A28="geotrace")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="108" priority="98" stopIfTrue="1">
-      <formula>OR($A15="audio audit", $A15="text audit", $A15="speed violations count", $A15="speed violations list", $A15="speed violations audit")</formula>
+      <formula>OR($A28="audio audit", $A28="text audit", $A28="speed violations count", $A28="speed violations list", $A28="speed violations audit")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="107" priority="99" stopIfTrue="1">
-      <formula>OR($A15="username", $A15="phonenumber", $A15="start", $A15="end", $A15="deviceid", $A15="subscriberid", $A15="simserial", $A15="caseid")</formula>
+      <formula>OR($A28="username", $A28="phonenumber", $A28="start", $A28="end", $A28="deviceid", $A28="subscriberid", $A28="simserial", $A28="caseid")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="106" priority="100" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A15, 16)="select_multiple ", LEN($A15)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A15, 17)))), AND(LEFT($A15, 11)="select_one ", LEN($A15)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A15, 12)))))</formula>
+      <formula>OR(AND(LEFT($A28, 16)="select_multiple ", LEN($A28)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A28, 17)))), AND(LEFT($A28, 11)="select_one ", LEN($A28)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A28, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="105" priority="102" stopIfTrue="1">
-      <formula>$A15="decimal"</formula>
+      <formula>$A28="decimal"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="104" priority="104" stopIfTrue="1">
-      <formula>$A15="integer"</formula>
+      <formula>$A28="integer"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="103" priority="106" stopIfTrue="1">
-      <formula>$A15="text"</formula>
+      <formula>$A28="text"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="102" priority="107" stopIfTrue="1">
-      <formula>$A15="end repeat"</formula>
+      <formula>$A28="end repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="101" priority="108" stopIfTrue="1">
-      <formula>$A15="begin repeat"</formula>
+      <formula>$A28="begin repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="100" priority="109" stopIfTrue="1">
-      <formula>$A15="end group"</formula>
+      <formula>$A28="end group"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="99" priority="110" stopIfTrue="1">
-      <formula>$A15="begin group"</formula>
+      <formula>$A28="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -6212,11 +6536,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6228,7 +6552,7 @@
     <col min="6" max="16384" width="10.83203125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
@@ -6245,7 +6569,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
@@ -6256,7 +6580,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>21</v>
       </c>
@@ -6267,34 +6591,189 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>413</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>378</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>414</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>378</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>415</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>416</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>378</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>417</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -6306,7 +6785,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H2000">
+  <conditionalFormatting sqref="A2:H4 A10:H2000">
     <cfRule type="expression" dxfId="98" priority="1">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
@@ -6322,7 +6801,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6358,14 +6837,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>382</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>383</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2111231643</v>
+        <v>2111301608</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>

</xml_diff>